<commit_message>
update res_mat and tabular
</commit_message>
<xml_diff>
--- a/tests.xlsx
+++ b/tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="28">
   <si>
     <t>Operation</t>
   </si>
@@ -78,9 +78,6 @@
     <t>O0</t>
   </si>
   <si>
-    <t>double</t>
-  </si>
-  <si>
     <t>550*550</t>
   </si>
   <si>
@@ -88,6 +85,24 @@
   </si>
   <si>
     <t>Vectorisation</t>
+  </si>
+  <si>
+    <t>Addition small</t>
+  </si>
+  <si>
+    <t>Addition big</t>
+  </si>
+  <si>
+    <t>Multiplication small</t>
+  </si>
+  <si>
+    <t>Multiplication big</t>
+  </si>
+  <si>
+    <t>Gain avec openMp</t>
+  </si>
+  <si>
+    <t>Gain en %</t>
   </si>
 </sst>
 </file>
@@ -149,7 +164,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -203,14 +218,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="55">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -237,6 +255,7 @@
     <cellStyle name="Lien hypertexte" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -263,9 +282,19 @@
     <cellStyle name="Lien hypertexte visité" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -282,12 +311,6 @@
         <name val="Zapf Dingbats"/>
         <scheme val="none"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -312,21 +335,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:M25" totalsRowShown="0">
-  <autoFilter ref="A1:M25"/>
-  <sortState ref="A2:M25">
-    <sortCondition descending="1" ref="M1:M25"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:M13" totalsRowShown="0">
+  <sortState ref="A2:M13">
+    <sortCondition descending="1" ref="M1:M13"/>
   </sortState>
   <tableColumns count="13">
     <tableColumn id="1" name="Operation"/>
-    <tableColumn id="2" name="OpenMp" dataDxfId="3"/>
-    <tableColumn id="13" name="Vectorisation" dataDxfId="0"/>
+    <tableColumn id="2" name="OpenMp" dataDxfId="4"/>
+    <tableColumn id="13" name="Vectorisation" dataDxfId="3"/>
     <tableColumn id="3" name="Option compilation"/>
     <tableColumn id="4" name="Taille de la matrice"/>
     <tableColumn id="5" name="variable(type)"/>
     <tableColumn id="6" name="Temps exec (m)" dataDxfId="2"/>
     <tableColumn id="7" name="Temps exec (s)"/>
-    <tableColumn id="8" name="Temps total adapté (s)" dataDxfId="1">
+    <tableColumn id="8" name="Temps total adapté (s)" dataDxfId="0">
       <calculatedColumnFormula>(60*G2)/4+(H2/4)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" name="Nombre total de calculs"/>
@@ -339,6 +361,17 @@
     <tableColumn id="12" name="Gflops">
       <calculatedColumnFormula>L2/1000</calculatedColumnFormula>
     </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="I15:J19" totalsRowShown="0">
+  <autoFilter ref="I15:J19"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Gain avec openMp"/>
+    <tableColumn id="2" name="Gain en %" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -666,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -682,7 +715,7 @@
     <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="16.33203125" customWidth="1"/>
     <col min="9" max="9" width="21.6640625" customWidth="1"/>
-    <col min="10" max="10" width="23.1640625" customWidth="1"/>
+    <col min="10" max="10" width="21.83203125" customWidth="1"/>
     <col min="11" max="11" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -694,7 +727,7 @@
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -729,7 +762,7 @@
     </row>
     <row r="2" spans="1:13">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>7</v>
@@ -738,38 +771,38 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
         <v>14</v>
       </c>
       <c r="G2" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H2">
-        <v>9.0760000000000005</v>
+        <v>12.771000000000001</v>
       </c>
       <c r="I2">
         <f>(60*G2)/4+(H2/4)</f>
-        <v>2.2690000000000001</v>
+        <v>63.192750000000004</v>
       </c>
       <c r="J2">
-        <v>9922500000</v>
+        <v>166375000000</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K25" si="0">J2/I2</f>
-        <v>4373071837.8140144</v>
+        <f>J2/I2</f>
+        <v>2632817846.9840288</v>
       </c>
       <c r="L2">
-        <f t="shared" ref="L2:L25" si="1">K2/1000000</f>
-        <v>4373.0718378140145</v>
+        <f>K2/1000000</f>
+        <v>2632.8178469840286</v>
       </c>
       <c r="M2">
-        <f t="shared" ref="M2:M25" si="2">L2/1000</f>
-        <v>4.373071837814015</v>
+        <f>L2/1000</f>
+        <v>2.6328178469840284</v>
       </c>
     </row>
     <row r="3" spans="1:13">
@@ -783,10 +816,10 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
@@ -795,26 +828,26 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>31.346</v>
+        <v>46.558999999999997</v>
       </c>
       <c r="I3">
         <f>(60*G3)/4+(H3/4)</f>
-        <v>7.8365</v>
+        <v>11.639749999999999</v>
       </c>
       <c r="J3">
         <v>30250000000</v>
       </c>
       <c r="K3">
-        <f t="shared" si="0"/>
-        <v>3860141644.8669686</v>
+        <f>J3/I3</f>
+        <v>2598853068.1500893</v>
       </c>
       <c r="L3">
-        <f t="shared" si="1"/>
-        <v>3860.1416448669688</v>
+        <f>K3/1000000</f>
+        <v>2598.8530681500893</v>
       </c>
       <c r="M3">
-        <f t="shared" si="2"/>
-        <v>3.8601416448669688</v>
+        <f>L3/1000</f>
+        <v>2.5988530681500892</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -828,7 +861,7 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
         <v>13</v>
@@ -840,31 +873,31 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>34.325000000000003</v>
+        <v>50.55</v>
       </c>
       <c r="I4">
         <f>(60*G4)/4+(H4/4)</f>
-        <v>8.5812500000000007</v>
+        <v>12.637499999999999</v>
       </c>
       <c r="J4">
         <v>31255875000</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
-        <v>3642345229.4246173</v>
+        <f>J4/I4</f>
+        <v>2473264094.9554896</v>
       </c>
       <c r="L4">
-        <f t="shared" si="1"/>
-        <v>3642.3452294246172</v>
+        <f>K4/1000000</f>
+        <v>2473.2640949554898</v>
       </c>
       <c r="M4">
-        <f t="shared" si="2"/>
-        <v>3.6423452294246172</v>
+        <f>L4/1000</f>
+        <v>2.4732640949554896</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>7</v>
@@ -873,218 +906,218 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G5" s="2">
         <v>0</v>
       </c>
       <c r="H5">
-        <v>44.557000000000002</v>
+        <v>33.1</v>
       </c>
       <c r="I5">
         <f>(60*G5)/4+(H5/4)</f>
-        <v>11.139250000000001</v>
+        <v>8.2750000000000004</v>
       </c>
       <c r="J5">
-        <v>31255875000</v>
+        <v>9922500000</v>
       </c>
       <c r="K5">
-        <f t="shared" si="0"/>
-        <v>2805922750.6340194</v>
+        <f>J5/I5</f>
+        <v>1199093655.5891237</v>
       </c>
       <c r="L5">
-        <f t="shared" si="1"/>
-        <v>2805.9227506340194</v>
+        <f>K5/1000000</f>
+        <v>1199.0936555891237</v>
       </c>
       <c r="M5">
-        <f t="shared" si="2"/>
-        <v>2.8059227506340192</v>
+        <f>L5/1000</f>
+        <v>1.1990936555891236</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
+      <c r="B6" t="s">
+        <v>8</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G6" s="2">
         <v>0</v>
       </c>
       <c r="H6">
-        <v>16.742999999999999</v>
+        <v>11.632</v>
       </c>
       <c r="I6">
-        <f>(60*G6)/4+(H6/4)</f>
-        <v>4.1857499999999996</v>
+        <f>(60*G6)+(H6)</f>
+        <v>11.632</v>
       </c>
       <c r="J6">
         <v>9922500000</v>
       </c>
       <c r="K6">
-        <f t="shared" si="0"/>
-        <v>2370542913.4563699</v>
+        <f>J6/I6</f>
+        <v>853034731.77441537</v>
       </c>
       <c r="L6">
-        <f t="shared" si="1"/>
-        <v>2370.5429134563697</v>
+        <f>K6/1000000</f>
+        <v>853.03473177441538</v>
       </c>
       <c r="M6">
-        <f t="shared" si="2"/>
-        <v>2.3705429134563696</v>
+        <f>L6/1000</f>
+        <v>0.85303473177441536</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="2">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="H7">
-        <v>4.79</v>
+        <v>46.323</v>
       </c>
       <c r="I7">
-        <f>(60*G7)+(H7)</f>
-        <v>4.79</v>
+        <f>(60*G7)/4+(H7/4)</f>
+        <v>206.58074999999999</v>
       </c>
       <c r="J7">
-        <v>9922500000</v>
+        <v>166375000000</v>
       </c>
       <c r="K7">
-        <f t="shared" si="0"/>
-        <v>2071503131.5240083</v>
+        <f>J7/I7</f>
+        <v>805375137.80930698</v>
       </c>
       <c r="L7">
-        <f t="shared" si="1"/>
-        <v>2071.5031315240085</v>
+        <f>K7/1000000</f>
+        <v>805.37513780930703</v>
       </c>
       <c r="M7">
-        <f t="shared" si="2"/>
-        <v>2.0715031315240084</v>
+        <f>L7/1000</f>
+        <v>0.80537513780930703</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
+      <c r="B8" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F8" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H8">
-        <v>8.6660000000000004</v>
+        <v>45.661999999999999</v>
       </c>
       <c r="I8">
-        <f>(60*G8)/4+(H8/4)</f>
-        <v>92.166499999999999</v>
+        <f>(60*G8)+(H8)</f>
+        <v>225.66200000000001</v>
       </c>
       <c r="J8">
         <v>166375000000</v>
       </c>
       <c r="K8">
-        <f t="shared" si="0"/>
-        <v>1805156971.3507619</v>
+        <f>J8/I8</f>
+        <v>737275216.91733658</v>
       </c>
       <c r="L8">
-        <f t="shared" si="1"/>
-        <v>1805.156971350762</v>
+        <f>K8/1000000</f>
+        <v>737.27521691733659</v>
       </c>
       <c r="M8">
-        <f t="shared" si="2"/>
-        <v>1.805156971350762</v>
+        <f>L8/1000</f>
+        <v>0.73727521691733655</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F9" t="s">
         <v>14</v>
       </c>
       <c r="G9" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H9">
-        <v>17.062999999999999</v>
+        <v>57.704999999999998</v>
       </c>
       <c r="I9">
-        <f>(60*G9)+(H9)</f>
-        <v>17.062999999999999</v>
+        <f>(60*G9)/4+(H9/4)</f>
+        <v>44.426249999999996</v>
       </c>
       <c r="J9">
-        <v>30250000000</v>
+        <v>31255875000</v>
       </c>
       <c r="K9">
-        <f t="shared" si="0"/>
-        <v>1772841821.4850848</v>
+        <f>J9/I9</f>
+        <v>703545201.31678915</v>
       </c>
       <c r="L9">
-        <f t="shared" si="1"/>
-        <v>1772.8418214850847</v>
+        <f>K9/1000000</f>
+        <v>703.54520131678919</v>
       </c>
       <c r="M9">
-        <f t="shared" si="2"/>
-        <v>1.7728418214850847</v>
+        <f>L9/1000</f>
+        <v>0.70354520131678921</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -1098,7 +1131,7 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E10" t="s">
         <v>13</v>
@@ -1110,31 +1143,31 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>19.648</v>
+        <v>51.167000000000002</v>
       </c>
       <c r="I10">
         <f>(60*G10)+(H10)</f>
-        <v>19.648</v>
+        <v>51.167000000000002</v>
       </c>
       <c r="J10">
         <v>31255875000</v>
       </c>
       <c r="K10">
-        <f t="shared" si="0"/>
-        <v>1590791683.6319218</v>
+        <f>J10/I10</f>
+        <v>610860026.97050834</v>
       </c>
       <c r="L10">
-        <f t="shared" si="1"/>
-        <v>1590.7916836319218</v>
+        <f>K10/1000000</f>
+        <v>610.86002697050833</v>
       </c>
       <c r="M10">
-        <f t="shared" si="2"/>
-        <v>1.5907916836319218</v>
+        <f>L10/1000</f>
+        <v>0.61086002697050834</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>8</v>
@@ -1143,675 +1176,180 @@
         <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F11" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>19.817</v>
+        <v>13.504</v>
       </c>
       <c r="I11">
         <f>(60*G11)+(H11)</f>
-        <v>19.817</v>
+        <v>73.504000000000005</v>
       </c>
       <c r="J11">
-        <v>31255875000</v>
+        <v>30250000000</v>
       </c>
       <c r="K11">
-        <f t="shared" si="0"/>
-        <v>1577225362.0628753</v>
+        <f>J11/I11</f>
+        <v>411542228.99434042</v>
       </c>
       <c r="L11">
-        <f t="shared" si="1"/>
-        <v>1577.2253620628753</v>
+        <f>K11/1000000</f>
+        <v>411.54222899434041</v>
       </c>
       <c r="M11">
-        <f t="shared" si="2"/>
-        <v>1.5772253620628753</v>
+        <f>L11/1000</f>
+        <v>0.4115422289943404</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>8</v>
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C12" t="s">
         <v>8</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F12" t="s">
         <v>14</v>
       </c>
       <c r="G12" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H12">
-        <v>48.969000000000001</v>
+        <v>44.4</v>
       </c>
       <c r="I12">
-        <f>(60*G12)+(H12)</f>
-        <v>108.96899999999999</v>
+        <f>(60*G12)/4+(H12/4)</f>
+        <v>86.1</v>
       </c>
       <c r="J12">
-        <v>166375000000</v>
+        <v>30250000000</v>
       </c>
       <c r="K12">
-        <f t="shared" si="0"/>
-        <v>1526810377.2632585</v>
+        <f>J12/I12</f>
+        <v>351335656.213705</v>
       </c>
       <c r="L12">
-        <f t="shared" si="1"/>
-        <v>1526.8103772632585</v>
+        <f>K12/1000000</f>
+        <v>351.33565621370502</v>
       </c>
       <c r="M12">
-        <f t="shared" si="2"/>
-        <v>1.5268103772632584</v>
+        <f>L12/1000</f>
+        <v>0.35133565621370499</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>8</v>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E13" t="s">
         <v>13</v>
       </c>
       <c r="F13" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="G13" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H13">
-        <v>9.0079999999999991</v>
+        <v>12.648</v>
       </c>
       <c r="I13">
-        <f>(60*G13)+(H13)</f>
-        <v>9.0079999999999991</v>
+        <f>(60*G13)/4+(H13/4)</f>
+        <v>33.161999999999999</v>
       </c>
       <c r="J13">
         <v>9922500000</v>
       </c>
       <c r="K13">
-        <f t="shared" si="0"/>
-        <v>1101520870.3374779</v>
+        <f>J13/I13</f>
+        <v>299212954.58657503</v>
       </c>
       <c r="L13">
-        <f t="shared" si="1"/>
-        <v>1101.5208703374778</v>
+        <f>K13/1000000</f>
+        <v>299.21295458657505</v>
       </c>
       <c r="M13">
-        <f t="shared" si="2"/>
-        <v>1.1015208703374779</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="2">
-        <v>2</v>
-      </c>
-      <c r="H14">
-        <v>5.9039999999999999</v>
-      </c>
-      <c r="I14">
-        <f>(60*G14)/4+(H14/4)</f>
-        <v>31.475999999999999</v>
-      </c>
-      <c r="J14">
-        <v>31255875000</v>
-      </c>
-      <c r="K14">
-        <f t="shared" si="0"/>
-        <v>993006576.43919182</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="1"/>
-        <v>993.0065764391918</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="2"/>
-        <v>0.99300657643919177</v>
+        <f>L13/1000</f>
+        <v>0.29921295458657504</v>
       </c>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="2">
-        <v>12</v>
-      </c>
-      <c r="H15">
-        <v>3.343</v>
-      </c>
-      <c r="I15">
-        <f>(60*G15)/4+(H15/4)</f>
-        <v>180.83574999999999</v>
-      </c>
-      <c r="J15">
-        <v>166375000000</v>
-      </c>
-      <c r="K15">
-        <f t="shared" si="0"/>
-        <v>920033787.56689429</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="1"/>
-        <v>920.03378756689426</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="2"/>
-        <v>0.92003378756689425</v>
+      <c r="I15" t="s">
+        <v>26</v>
+      </c>
+      <c r="J15" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" s="2">
-        <v>2</v>
-      </c>
-      <c r="H16">
-        <v>21.936</v>
-      </c>
-      <c r="I16">
-        <f>(60*G16)/4+(H16/4)</f>
-        <v>35.484000000000002</v>
-      </c>
-      <c r="J16">
-        <v>30250000000</v>
-      </c>
-      <c r="K16">
-        <f t="shared" si="0"/>
-        <v>852496900.01127267</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="1"/>
-        <v>852.49690001127271</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="2"/>
-        <v>0.85249690001127276</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" t="s">
-        <v>19</v>
-      </c>
-      <c r="G17" s="2">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>50.347999999999999</v>
-      </c>
-      <c r="I17">
-        <f>(60*G17)+(H17)</f>
-        <v>50.347999999999999</v>
-      </c>
-      <c r="J17">
-        <v>30250000000</v>
-      </c>
-      <c r="K17">
-        <f t="shared" si="0"/>
-        <v>600818304.59998417</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="1"/>
-        <v>600.81830459998412</v>
-      </c>
-      <c r="M17">
-        <f t="shared" si="2"/>
-        <v>0.60081830459998409</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G18" s="2">
-        <v>19</v>
-      </c>
-      <c r="H18">
-        <v>21.622</v>
-      </c>
-      <c r="I18">
-        <f>(60*G18)/4+(H18/4)</f>
-        <v>290.40550000000002</v>
-      </c>
-      <c r="J18">
-        <v>166375000000</v>
-      </c>
-      <c r="K18">
-        <f t="shared" si="0"/>
-        <v>572905816.17772388</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="1"/>
-        <v>572.90581617772386</v>
-      </c>
-      <c r="M18">
-        <f t="shared" si="2"/>
-        <v>0.57290581617772385</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" t="s">
-        <v>13</v>
-      </c>
-      <c r="F19" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="2">
-        <v>1</v>
-      </c>
-      <c r="H19">
-        <v>12.03</v>
-      </c>
-      <c r="I19">
-        <f>(60*G19)/4+(H19/4)</f>
-        <v>18.0075</v>
-      </c>
-      <c r="J19">
-        <v>9922500000</v>
-      </c>
-      <c r="K19">
-        <f t="shared" si="0"/>
-        <v>551020408.16326535</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="1"/>
-        <v>551.0204081632653</v>
-      </c>
-      <c r="M19">
-        <f t="shared" si="2"/>
-        <v>0.55102040816326525</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G20" s="2">
-        <v>1</v>
-      </c>
-      <c r="H20">
-        <v>15.169</v>
-      </c>
-      <c r="I20">
-        <f>(60*G20)/4+(H20/4)</f>
-        <v>18.792249999999999</v>
-      </c>
-      <c r="J20">
-        <v>9922500000</v>
-      </c>
-      <c r="K20">
-        <f t="shared" si="0"/>
-        <v>528010216.97774351</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="1"/>
-        <v>528.01021697774354</v>
-      </c>
-      <c r="M20">
-        <f t="shared" si="2"/>
-        <v>0.52801021697774353</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" t="s">
-        <v>14</v>
-      </c>
-      <c r="G21" s="2">
-        <v>3</v>
-      </c>
-      <c r="H21">
-        <v>56.414999999999999</v>
-      </c>
-      <c r="I21">
-        <f>(60*G21)/4+(H21/4)</f>
-        <v>59.103749999999998</v>
-      </c>
-      <c r="J21">
-        <v>30250000000</v>
-      </c>
-      <c r="K21">
-        <f t="shared" si="0"/>
-        <v>511811856.26969528</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="1"/>
-        <v>511.81185626969528</v>
-      </c>
-      <c r="M21">
-        <f t="shared" si="2"/>
-        <v>0.51181185626969528</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13">
-      <c r="A22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" t="s">
-        <v>19</v>
-      </c>
-      <c r="G22" s="2">
-        <v>4</v>
-      </c>
-      <c r="H22">
-        <v>16.280999999999999</v>
-      </c>
-      <c r="I22">
-        <f>(60*G22)/4+(H22/4)</f>
-        <v>64.070250000000001</v>
-      </c>
-      <c r="J22">
-        <v>30250000000</v>
-      </c>
-      <c r="K22">
-        <f t="shared" si="0"/>
-        <v>472138004.76820362</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="1"/>
-        <v>472.13800476820364</v>
-      </c>
-      <c r="M22">
-        <f t="shared" si="2"/>
-        <v>0.47213800476820367</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="A23" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" t="s">
-        <v>20</v>
-      </c>
-      <c r="F23" t="s">
-        <v>19</v>
-      </c>
-      <c r="G23" s="2">
-        <v>5</v>
-      </c>
-      <c r="H23">
-        <v>54.124000000000002</v>
-      </c>
-      <c r="I23">
-        <f>(60*G23)+(H23)</f>
-        <v>354.12400000000002</v>
-      </c>
-      <c r="J23">
-        <v>166375000000</v>
-      </c>
-      <c r="K23">
-        <f t="shared" si="0"/>
-        <v>469821305.53139573</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="1"/>
-        <v>469.82130553139575</v>
-      </c>
-      <c r="M23">
-        <f t="shared" si="2"/>
-        <v>0.46982130553139573</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24" t="s">
-        <v>13</v>
-      </c>
-      <c r="F24" t="s">
-        <v>19</v>
-      </c>
-      <c r="G24" s="2">
-        <v>6</v>
-      </c>
-      <c r="H24">
-        <v>29.021000000000001</v>
-      </c>
-      <c r="I24">
-        <f>(60*G24)/4+(H24/4)</f>
-        <v>97.255250000000004</v>
-      </c>
-      <c r="J24">
-        <v>31255875000</v>
-      </c>
-      <c r="K24">
-        <f t="shared" si="0"/>
-        <v>321379822.6830942</v>
-      </c>
-      <c r="L24">
-        <f t="shared" si="1"/>
-        <v>321.37982268309418</v>
-      </c>
-      <c r="M24">
-        <f t="shared" si="2"/>
-        <v>0.32137982268309417</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13">
-      <c r="A25" t="s">
-        <v>9</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" t="s">
-        <v>18</v>
-      </c>
-      <c r="E25" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25" s="2">
-        <v>41</v>
-      </c>
-      <c r="H25">
-        <v>8.3610000000000007</v>
-      </c>
-      <c r="I25">
-        <f>(60*G25)/4+(H25/4)</f>
-        <v>617.09024999999997</v>
-      </c>
-      <c r="J25">
-        <v>166375000000</v>
-      </c>
-      <c r="K25">
-        <f t="shared" si="0"/>
-        <v>269612102.9298389</v>
-      </c>
-      <c r="L25">
-        <f t="shared" si="1"/>
-        <v>269.6121029298389</v>
-      </c>
-      <c r="M25">
-        <f t="shared" si="2"/>
-        <v>0.26961210292983889</v>
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="4">
+        <f>K5/K6-1</f>
+        <v>0.40567975830815706</v>
+      </c>
+    </row>
+    <row r="17" spans="9:10">
+      <c r="I17" t="s">
+        <v>23</v>
+      </c>
+      <c r="J17" s="4">
+        <f>K3/K11-1</f>
+        <v>5.314912261861295</v>
+      </c>
+    </row>
+    <row r="18" spans="9:10">
+      <c r="I18" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="4">
+        <f>K4/K10-1</f>
+        <v>3.0488229475766566</v>
+      </c>
+    </row>
+    <row r="19" spans="9:10">
+      <c r="I19" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" s="4">
+        <f>K2/K8-1</f>
+        <v>2.5710109150179408</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>